<commit_message>
Will wanted some files.
</commit_message>
<xml_diff>
--- a/LOOK.HERE_COUNT.xlsx
+++ b/LOOK.HERE_COUNT.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rmoge\GitHub\MuriSam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EEA33026-658E-407D-A5CC-FEB9326B5942}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D36113DA-BC2C-4DBB-B76A-26A14E458F88}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240"/>
+    <workbookView xWindow="23730" yWindow="8895" windowWidth="25725" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LOOK.HERE_COUNT" sheetId="1" r:id="rId1"/>
@@ -403,7 +403,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1238,11 +1238,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DT2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CU1" workbookViewId="0">
-      <selection activeCell="CY1" sqref="CY1:CY1048576"/>
+    <sheetView tabSelected="1" topLeftCell="BA1" workbookViewId="0">
+      <selection activeCell="BB2" sqref="BB2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1269,6 +1269,8 @@
     <col min="61" max="61" width="35" style="1" customWidth="1"/>
     <col min="65" max="65" width="36.28515625" customWidth="1"/>
     <col min="66" max="66" width="45.140625" customWidth="1"/>
+    <col min="67" max="67" width="31.85546875" customWidth="1"/>
+    <col min="68" max="68" width="37" customWidth="1"/>
     <col min="73" max="73" width="24.7109375" customWidth="1"/>
     <col min="74" max="74" width="27.85546875" customWidth="1"/>
     <col min="75" max="75" width="42" customWidth="1"/>

</xml_diff>